<commit_message>
Update final test suite.
</commit_message>
<xml_diff>
--- a/testing/webTestSuite.xlsx
+++ b/testing/webTestSuite.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\3\Pasca Emil\news-website\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95FD7318-8837-4FE7-8823-6011ABF0A52E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989E4EAD-F1D4-4D68-BAC7-0AE5A3AFEF77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17160" yWindow="5625" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foaie1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="115">
   <si>
     <t>#</t>
   </si>
@@ -376,7 +376,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -384,8 +384,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -395,6 +403,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -411,12 +437,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -701,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="D110" sqref="D110"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -716,34 +751,34 @@
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
-        <v>1</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="3" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>1</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>10</v>
       </c>
     </row>
@@ -775,11 +810,11 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
-        <v>2</v>
-      </c>
-      <c r="B6" s="1" t="s">
+    <row r="6" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="5">
+        <v>2</v>
+      </c>
+      <c r="B6" s="5" t="s">
         <v>15</v>
       </c>
     </row>
@@ -793,7 +828,7 @@
       <c r="D7" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -807,7 +842,7 @@
       <c r="D8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -821,15 +856,15 @@
       <c r="D9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>3</v>
-      </c>
-      <c r="B10" s="1" t="s">
+      <c r="G9" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>3</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>16</v>
       </c>
     </row>
@@ -843,9 +878,6 @@
       <c r="D11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="1">
@@ -857,7 +889,7 @@
       <c r="D12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -871,15 +903,15 @@
       <c r="D13" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="G13" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="5">
         <v>4</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="5" t="s">
         <v>20</v>
       </c>
     </row>
@@ -893,7 +925,7 @@
       <c r="D15" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G15" s="1" t="s">
+      <c r="G15" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -907,7 +939,7 @@
       <c r="D16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -921,7 +953,7 @@
       <c r="D17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -935,15 +967,15 @@
       <c r="D18" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="G18" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
         <v>5</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="5" t="s">
         <v>29</v>
       </c>
     </row>
@@ -957,7 +989,7 @@
       <c r="D20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -971,10 +1003,10 @@
       <c r="D21" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" s="3" t="s">
         <v>81</v>
       </c>
     </row>
@@ -988,15 +1020,15 @@
       <c r="D22" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="G22" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="5">
         <v>6</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="B23" s="5" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1010,7 +1042,7 @@
       <c r="D24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G24" s="1" t="s">
+      <c r="G24" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1024,7 +1056,7 @@
       <c r="D25" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G25" s="1" t="s">
+      <c r="G25" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1038,7 +1070,7 @@
       <c r="D26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G26" s="1" t="s">
+      <c r="G26" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1052,15 +1084,15 @@
       <c r="D27" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G27" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>7</v>
-      </c>
-      <c r="B28" s="1" t="s">
+      <c r="G27" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="5">
+        <v>7</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1074,7 +1106,7 @@
       <c r="D29" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G29" s="1" t="s">
+      <c r="G29" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1088,7 +1120,7 @@
       <c r="D30" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="G30" s="1" t="s">
+      <c r="G30" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1102,15 +1134,15 @@
       <c r="D31" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G31" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
-        <v>8</v>
-      </c>
-      <c r="B32" s="1" t="s">
+      <c r="G31" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="5">
+        <v>8</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1124,7 +1156,7 @@
       <c r="D33" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G33" s="1" t="s">
+      <c r="G33" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1138,7 +1170,7 @@
       <c r="D34" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="G34" s="1" t="s">
+      <c r="G34" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1152,7 +1184,7 @@
       <c r="D35" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="G35" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1166,15 +1198,15 @@
       <c r="D36" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G36" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+      <c r="G36" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="5">
         <v>9</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B37" s="5" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1188,7 +1220,7 @@
       <c r="D38" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G38" s="1" t="s">
+      <c r="G38" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1202,7 +1234,7 @@
       <c r="D39" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="G39" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1216,15 +1248,15 @@
       <c r="D40" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G40" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
+      <c r="G40" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="5">
         <v>10</v>
       </c>
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="5" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1238,7 +1270,7 @@
       <c r="D42" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G42" s="1" t="s">
+      <c r="G42" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1252,7 +1284,7 @@
       <c r="D43" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="G43" s="1" t="s">
+      <c r="G43" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1266,7 +1298,7 @@
       <c r="D44" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G44" s="1" t="s">
+      <c r="G44" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1280,15 +1312,15 @@
       <c r="D45" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G45" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="1">
+      <c r="G45" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="5">
         <v>11</v>
       </c>
-      <c r="B46" s="1" t="s">
+      <c r="B46" s="5" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1302,7 +1334,7 @@
       <c r="D47" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G47" s="1" t="s">
+      <c r="G47" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1316,7 +1348,7 @@
       <c r="D48" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G48" s="1" t="s">
+      <c r="G48" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1330,15 +1362,15 @@
       <c r="D49" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G49" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="1">
+      <c r="G49" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="5">
         <v>12</v>
       </c>
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="5" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1352,7 +1384,7 @@
       <c r="D51" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G51" s="1" t="s">
+      <c r="G51" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1366,7 +1398,7 @@
       <c r="D52" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="G52" s="1" t="s">
+      <c r="G52" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1380,7 +1412,7 @@
       <c r="D53" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G53" s="1" t="s">
+      <c r="G53" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1394,15 +1426,15 @@
       <c r="D54" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="G54" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="1">
+      <c r="G54" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="5">
         <v>13</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="B55" s="5" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1416,7 +1448,7 @@
       <c r="D56" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G56" s="1" t="s">
+      <c r="G56" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1430,7 +1462,7 @@
       <c r="D57" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="G57" s="1" t="s">
+      <c r="G57" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1444,15 +1476,15 @@
       <c r="D58" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G58" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" s="1">
+      <c r="G58" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="5">
         <v>14</v>
       </c>
-      <c r="B59" s="1" t="s">
+      <c r="B59" s="5" t="s">
         <v>68</v>
       </c>
     </row>
@@ -1466,7 +1498,7 @@
       <c r="D60" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G60" s="1" t="s">
+      <c r="G60" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1480,7 +1512,7 @@
       <c r="D61" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="G61" s="1" t="s">
+      <c r="G61" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1494,7 +1526,7 @@
       <c r="D62" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G62" s="1" t="s">
+      <c r="G62" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1508,15 +1540,15 @@
       <c r="D63" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G63" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A64" s="1">
+      <c r="G63" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="5">
         <v>15</v>
       </c>
-      <c r="B64" s="1" t="s">
+      <c r="B64" s="5" t="s">
         <v>73</v>
       </c>
     </row>
@@ -1530,7 +1562,7 @@
       <c r="D65" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G65" s="1" t="s">
+      <c r="G65" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1544,7 +1576,7 @@
       <c r="D66" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="G66" s="1" t="s">
+      <c r="G66" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1558,15 +1590,15 @@
       <c r="D67" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G67" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="1">
+      <c r="G67" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="5">
         <v>16</v>
       </c>
-      <c r="B68" s="1" t="s">
+      <c r="B68" s="5" t="s">
         <v>76</v>
       </c>
     </row>
@@ -1580,7 +1612,7 @@
       <c r="D69" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G69" s="1" t="s">
+      <c r="G69" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1594,7 +1626,7 @@
       <c r="D70" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G70" s="1" t="s">
+      <c r="G70" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1608,7 +1640,7 @@
       <c r="D71" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G71" s="1" t="s">
+      <c r="G71" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1622,15 +1654,15 @@
       <c r="D72" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G72" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="1">
+      <c r="G72" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="5">
         <v>17</v>
       </c>
-      <c r="B73" s="1" t="s">
+      <c r="B73" s="5" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1644,7 +1676,7 @@
       <c r="D74" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G74" s="1" t="s">
+      <c r="G74" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1658,20 +1690,20 @@
       <c r="D75" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G75" s="1" t="s">
+      <c r="G75" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G76" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="1">
+      <c r="G76" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="5">
         <v>18</v>
       </c>
-      <c r="B77" s="1" t="s">
+      <c r="B77" s="5" t="s">
         <v>85</v>
       </c>
     </row>
@@ -1685,7 +1717,7 @@
       <c r="D78" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G78" s="1" t="s">
+      <c r="G78" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1699,7 +1731,7 @@
       <c r="D79" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G79" s="1" t="s">
+      <c r="G79" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1713,7 +1745,7 @@
       <c r="D80" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="G80" s="1" t="s">
+      <c r="G80" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1727,15 +1759,15 @@
       <c r="D81" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G81" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="82" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
+      <c r="G81" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="5">
         <v>19</v>
       </c>
-      <c r="B82" s="1" t="s">
+      <c r="B82" s="5" t="s">
         <v>92</v>
       </c>
     </row>
@@ -1749,6 +1781,9 @@
       <c r="D83" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="G83" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="84" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B84" s="1">
@@ -1760,6 +1795,9 @@
       <c r="D84" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="G84" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B85" s="1">
@@ -1770,6 +1808,9 @@
       </c>
       <c r="D85" s="1" t="s">
         <v>96</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="86" spans="1:7" ht="30" x14ac:dyDescent="0.25">
@@ -1782,12 +1823,15 @@
       <c r="D86" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="1">
+      <c r="G86" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="5">
         <v>20</v>
       </c>
-      <c r="B87" s="1" t="s">
+      <c r="B87" s="5" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1801,6 +1845,9 @@
       <c r="D88" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="G88" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="89" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B89" s="1">
@@ -1812,6 +1859,9 @@
       <c r="D89" s="1" t="s">
         <v>95</v>
       </c>
+      <c r="G89" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B90" s="1">
@@ -1822,6 +1872,9 @@
       </c>
       <c r="D90" s="1" t="s">
         <v>99</v>
+      </c>
+      <c r="G90" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
@@ -1834,12 +1887,15 @@
       <c r="D91" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A92" s="1">
+      <c r="G91" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A92" s="5">
         <v>21</v>
       </c>
-      <c r="B92" s="1" t="s">
+      <c r="B92" s="5" t="s">
         <v>100</v>
       </c>
     </row>
@@ -1853,6 +1909,9 @@
       <c r="D93" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="G93" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="94" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B94" s="1">
@@ -1864,6 +1923,9 @@
       <c r="D94" s="1" t="s">
         <v>90</v>
       </c>
+      <c r="G94" s="2" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="95" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B95" s="1">
@@ -1877,6 +1939,9 @@
       </c>
       <c r="E95" s="1" t="s">
         <v>105</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="96" spans="1:7" ht="45" x14ac:dyDescent="0.25">
@@ -1892,16 +1957,19 @@
       <c r="E96" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="97" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A97" s="1">
+      <c r="G96" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A97" s="5">
         <v>22</v>
       </c>
-      <c r="B97" s="1" t="s">
+      <c r="B97" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B98" s="1">
         <v>1</v>
       </c>
@@ -1911,8 +1979,11 @@
       <c r="D98" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="99" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="G98" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B99" s="1">
         <v>2</v>
       </c>
@@ -1922,8 +1993,11 @@
       <c r="D99" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="100" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="G99" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B100" s="1">
         <v>3</v>
       </c>
@@ -1936,8 +2010,11 @@
       <c r="E100" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="G100" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="B101" s="1">
         <v>4</v>
       </c>
@@ -1950,16 +2027,19 @@
       <c r="E101" s="1" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A102" s="1">
+      <c r="G101" s="3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A102" s="5">
         <v>23</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B102" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B103" s="1">
         <v>1</v>
       </c>
@@ -1969,8 +2049,11 @@
       <c r="D103" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="104" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="G103" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B104" s="1">
         <v>2</v>
       </c>
@@ -1980,8 +2063,11 @@
       <c r="D104" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G104" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B105" s="1">
         <v>3</v>
       </c>
@@ -1991,8 +2077,11 @@
       <c r="D105" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="106" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="G105" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="B106" s="1">
         <v>4</v>
       </c>
@@ -2002,16 +2091,19 @@
       <c r="D106" s="1" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A107" s="1">
+      <c r="G106" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="5">
         <v>24</v>
       </c>
-      <c r="B107" s="1" t="s">
+      <c r="B107" s="5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B108" s="1">
         <v>1</v>
       </c>
@@ -2021,8 +2113,11 @@
       <c r="D108" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G108" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B109" s="1">
         <v>2</v>
       </c>
@@ -2032,8 +2127,11 @@
       <c r="D109" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G109" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B110" s="1">
         <v>3</v>
       </c>
@@ -2042,6 +2140,9 @@
       </c>
       <c r="D110" s="1" t="s">
         <v>114</v>
+      </c>
+      <c r="G110" s="2" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>